<commit_message>
GANTT A JOUR !!!!
</commit_message>
<xml_diff>
--- a/lycee_java/project/Gantt.xlsx
+++ b/lycee_java/project/Gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38664446-BDF6-4501-8A03-E887555E3BC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5942FD3F-0A2F-4BC5-8EFB-2694AD84BF4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
   <si>
     <t>Créez un diagramme de Gantt dans cette feuille de calcul.
 Entrez le titre de ce projet dans la cellule B1. 
@@ -170,9 +170,6 @@
     <t>Gestion des sanctions</t>
   </si>
   <si>
-    <t>Rédation documentation</t>
-  </si>
-  <si>
     <t>QUENTIN &amp; AMINE</t>
   </si>
   <si>
@@ -186,6 +183,12 @@
   </si>
   <si>
     <t>Gestion des absences et retard des étudiants AVEC FORMULAIRE</t>
+  </si>
+  <si>
+    <t>QUENTIN / LOIC</t>
+  </si>
+  <si>
+    <t>Rédation documentation développeur</t>
   </si>
 </sst>
 </file>
@@ -1827,7 +1830,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="39" fmlaLink="$E$3" horiz="1" max="365" page="0" val="9"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="39" fmlaLink="$E$3" horiz="1" max="365" page="0" val="13"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2178,8 +2181,8 @@
   </sheetPr>
   <dimension ref="A1:BK25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2242,7 +2245,7 @@
       </c>
       <c r="D3" s="56"/>
       <c r="E3" s="33">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="H3" s="40"/>
       <c r="I3" s="41"/>
@@ -2356,227 +2359,227 @@
       <c r="G5" s="29"/>
       <c r="H5" s="43">
         <f ca="1">IFERROR(Début_Projet+Incrément_Défilement,TODAY())</f>
-        <v>44209</v>
+        <v>44213</v>
       </c>
       <c r="I5" s="44">
         <f ca="1">H5+1</f>
-        <v>44210</v>
+        <v>44214</v>
       </c>
       <c r="J5" s="45">
         <f t="shared" ref="J5:AW5" ca="1" si="0">I5+1</f>
-        <v>44211</v>
+        <v>44215</v>
       </c>
       <c r="K5" s="45">
         <f ca="1">J5+1</f>
-        <v>44212</v>
+        <v>44216</v>
       </c>
       <c r="L5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44213</v>
+        <v>44217</v>
       </c>
       <c r="M5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44214</v>
+        <v>44218</v>
       </c>
       <c r="N5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44215</v>
+        <v>44219</v>
       </c>
       <c r="O5" s="45">
         <f ca="1">N5+1</f>
-        <v>44216</v>
+        <v>44220</v>
       </c>
       <c r="P5" s="45">
         <f ca="1">O5+1</f>
-        <v>44217</v>
+        <v>44221</v>
       </c>
       <c r="Q5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44218</v>
+        <v>44222</v>
       </c>
       <c r="R5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44219</v>
+        <v>44223</v>
       </c>
       <c r="S5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44220</v>
+        <v>44224</v>
       </c>
       <c r="T5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44221</v>
+        <v>44225</v>
       </c>
       <c r="U5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44222</v>
+        <v>44226</v>
       </c>
       <c r="V5" s="45">
         <f ca="1">U5+1</f>
-        <v>44223</v>
+        <v>44227</v>
       </c>
       <c r="W5" s="45">
         <f ca="1">V5+1</f>
-        <v>44224</v>
+        <v>44228</v>
       </c>
       <c r="X5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44225</v>
+        <v>44229</v>
       </c>
       <c r="Y5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44226</v>
+        <v>44230</v>
       </c>
       <c r="Z5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44227</v>
+        <v>44231</v>
       </c>
       <c r="AA5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44228</v>
+        <v>44232</v>
       </c>
       <c r="AB5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44229</v>
+        <v>44233</v>
       </c>
       <c r="AC5" s="45">
         <f ca="1">AB5+1</f>
-        <v>44230</v>
+        <v>44234</v>
       </c>
       <c r="AD5" s="45">
         <f ca="1">AC5+1</f>
-        <v>44231</v>
+        <v>44235</v>
       </c>
       <c r="AE5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44232</v>
+        <v>44236</v>
       </c>
       <c r="AF5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44233</v>
+        <v>44237</v>
       </c>
       <c r="AG5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44234</v>
+        <v>44238</v>
       </c>
       <c r="AH5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44235</v>
+        <v>44239</v>
       </c>
       <c r="AI5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44236</v>
+        <v>44240</v>
       </c>
       <c r="AJ5" s="45">
         <f ca="1">AI5+1</f>
-        <v>44237</v>
+        <v>44241</v>
       </c>
       <c r="AK5" s="45">
         <f ca="1">AJ5+1</f>
-        <v>44238</v>
+        <v>44242</v>
       </c>
       <c r="AL5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44239</v>
+        <v>44243</v>
       </c>
       <c r="AM5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44240</v>
+        <v>44244</v>
       </c>
       <c r="AN5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44241</v>
+        <v>44245</v>
       </c>
       <c r="AO5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44242</v>
+        <v>44246</v>
       </c>
       <c r="AP5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44243</v>
+        <v>44247</v>
       </c>
       <c r="AQ5" s="45">
         <f ca="1">AP5+1</f>
-        <v>44244</v>
+        <v>44248</v>
       </c>
       <c r="AR5" s="45">
         <f ca="1">AQ5+1</f>
-        <v>44245</v>
+        <v>44249</v>
       </c>
       <c r="AS5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44246</v>
+        <v>44250</v>
       </c>
       <c r="AT5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44247</v>
+        <v>44251</v>
       </c>
       <c r="AU5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44248</v>
+        <v>44252</v>
       </c>
       <c r="AV5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44249</v>
+        <v>44253</v>
       </c>
       <c r="AW5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>44250</v>
+        <v>44254</v>
       </c>
       <c r="AX5" s="45">
         <f ca="1">AW5+1</f>
-        <v>44251</v>
+        <v>44255</v>
       </c>
       <c r="AY5" s="45">
         <f ca="1">AX5+1</f>
-        <v>44252</v>
+        <v>44256</v>
       </c>
       <c r="AZ5" s="45">
         <f t="shared" ref="AZ5:BD5" ca="1" si="1">AY5+1</f>
-        <v>44253</v>
+        <v>44257</v>
       </c>
       <c r="BA5" s="45">
         <f t="shared" ca="1" si="1"/>
-        <v>44254</v>
+        <v>44258</v>
       </c>
       <c r="BB5" s="45">
         <f t="shared" ca="1" si="1"/>
-        <v>44255</v>
+        <v>44259</v>
       </c>
       <c r="BC5" s="45">
         <f t="shared" ca="1" si="1"/>
-        <v>44256</v>
+        <v>44260</v>
       </c>
       <c r="BD5" s="45">
         <f t="shared" ca="1" si="1"/>
-        <v>44257</v>
+        <v>44261</v>
       </c>
       <c r="BE5" s="45">
         <f ca="1">BD5+1</f>
-        <v>44258</v>
+        <v>44262</v>
       </c>
       <c r="BF5" s="45">
         <f ca="1">BE5+1</f>
-        <v>44259</v>
+        <v>44263</v>
       </c>
       <c r="BG5" s="45">
         <f t="shared" ref="BG5:BK5" ca="1" si="2">BF5+1</f>
-        <v>44260</v>
+        <v>44264</v>
       </c>
       <c r="BH5" s="45">
         <f t="shared" ca="1" si="2"/>
-        <v>44261</v>
+        <v>44265</v>
       </c>
       <c r="BI5" s="45">
         <f t="shared" ca="1" si="2"/>
-        <v>44262</v>
+        <v>44266</v>
       </c>
       <c r="BJ5" s="45">
         <f t="shared" ca="1" si="2"/>
-        <v>44263</v>
+        <v>44267</v>
       </c>
       <c r="BK5" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>44264</v>
+        <v>44268</v>
       </c>
     </row>
     <row r="6" spans="1:63" ht="31.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -2601,227 +2604,227 @@
       <c r="G6" s="19"/>
       <c r="H6" s="36" t="str">
         <f t="shared" ref="H6:AM6" ca="1" si="3">LEFT(TEXT(H5,"jjj"),1)</f>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="I6" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>l</v>
       </c>
       <c r="J6" s="39" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="K6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="L6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>j</v>
       </c>
       <c r="M6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>v</v>
       </c>
       <c r="N6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>s</v>
       </c>
       <c r="O6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="P6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>l</v>
       </c>
       <c r="Q6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="R6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="S6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>j</v>
       </c>
       <c r="T6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>v</v>
       </c>
       <c r="U6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>s</v>
       </c>
       <c r="V6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="W6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>l</v>
       </c>
       <c r="X6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="Y6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="Z6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>j</v>
       </c>
       <c r="AA6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>v</v>
       </c>
       <c r="AB6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>s</v>
       </c>
       <c r="AC6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="AD6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>l</v>
       </c>
       <c r="AE6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="AF6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="AG6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>j</v>
       </c>
       <c r="AH6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>v</v>
       </c>
       <c r="AI6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>s</v>
       </c>
       <c r="AJ6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="AK6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>l</v>
       </c>
       <c r="AL6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="AM6" s="38" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="AN6" s="38" t="str">
         <f t="shared" ref="AN6:BK6" ca="1" si="4">LEFT(TEXT(AN5,"jjj"),1)</f>
-        <v>d</v>
+        <v>j</v>
       </c>
       <c r="AO6" s="38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>l</v>
+        <v>v</v>
       </c>
       <c r="AP6" s="38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>s</v>
       </c>
       <c r="AQ6" s="38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="AR6" s="38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>j</v>
+        <v>l</v>
       </c>
       <c r="AS6" s="38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="AT6" s="38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="AU6" s="38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>j</v>
       </c>
       <c r="AV6" s="38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>l</v>
+        <v>v</v>
       </c>
       <c r="AW6" s="38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>s</v>
       </c>
       <c r="AX6" s="38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="AY6" s="38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>j</v>
+        <v>l</v>
       </c>
       <c r="AZ6" s="38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="BA6" s="38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="BB6" s="38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>j</v>
       </c>
       <c r="BC6" s="38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>l</v>
+        <v>v</v>
       </c>
       <c r="BD6" s="38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>s</v>
       </c>
       <c r="BE6" s="38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="BF6" s="38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>j</v>
+        <v>l</v>
       </c>
       <c r="BG6" s="38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="BH6" s="38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="BI6" s="38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>j</v>
       </c>
       <c r="BJ6" s="38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>l</v>
+        <v>v</v>
       </c>
       <c r="BK6" s="38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>s</v>
       </c>
     </row>
     <row r="7" spans="1:63" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -3133,10 +3136,10 @@
         <v>30</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="22">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="E9" s="23">
         <v>44200</v>
@@ -3376,7 +3379,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="22">
         <v>0.8</v>
@@ -3385,7 +3388,7 @@
         <v>44207</v>
       </c>
       <c r="F10" s="42">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G10" s="18"/>
       <c r="H10" s="26" t="str">
@@ -4343,13 +4346,13 @@
         <v>25</v>
       </c>
       <c r="D14" s="22">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E14" s="23">
         <v>44222</v>
       </c>
       <c r="F14" s="42">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G14" s="18"/>
       <c r="H14" s="26" t="str">
@@ -4404,9 +4407,9 @@
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(T$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="U14" s="47">
+      <c r="U14" s="47" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(U$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="V14" s="47" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(V$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
@@ -4583,16 +4586,16 @@
         <v>33</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="22">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E15" s="23">
         <v>44222</v>
       </c>
       <c r="F15" s="42">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G15" s="18"/>
       <c r="H15" s="26" t="str">
@@ -4647,9 +4650,9 @@
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(T$5=$E15,$F15=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="U15" s="47">
+      <c r="U15" s="47" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(U$5=$E15,$F15=1),Marqueur_Jalon,"")),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="V15" s="47" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(V$5=$E15,$F15=1),Marqueur_Jalon,"")),"")</f>
@@ -5067,7 +5070,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="22">
         <v>0</v>
@@ -5311,11 +5314,13 @@
         <v>25</v>
       </c>
       <c r="D18" s="22">
-        <v>0</v>
-      </c>
-      <c r="E18" s="23"/>
+        <v>0.1</v>
+      </c>
+      <c r="E18" s="23">
+        <v>44228</v>
+      </c>
       <c r="F18" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="18"/>
       <c r="H18" s="26"/>
@@ -5381,14 +5386,16 @@
         <v>36</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D19" s="22">
-        <v>0</v>
-      </c>
-      <c r="E19" s="23"/>
+        <v>0.1</v>
+      </c>
+      <c r="E19" s="23">
+        <v>44228</v>
+      </c>
       <c r="F19" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="18"/>
       <c r="H19" s="26"/>
@@ -5451,14 +5458,12 @@
     <row r="20" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="11"/>
       <c r="B20" s="48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="22">
-        <v>0</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D20" s="22"/>
       <c r="E20" s="23"/>
       <c r="F20" s="42">
         <v>0</v>
@@ -5530,14 +5535,16 @@
         <v>37</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" s="22">
-        <v>0</v>
-      </c>
-      <c r="E21" s="23"/>
+        <v>0.1</v>
+      </c>
+      <c r="E21" s="23">
+        <v>44228</v>
+      </c>
       <c r="F21" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="18"/>
       <c r="H21" s="26"/>
@@ -5600,10 +5607,10 @@
     <row r="22" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="11"/>
       <c r="B22" s="48" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" s="22">
         <v>0</v>
@@ -5676,7 +5683,7 @@
         <v>26</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="22">
         <v>0</v>

</xml_diff>